<commit_message>
Control de excepciones y comentar codigo
</commit_message>
<xml_diff>
--- a/Archivos_xlsx/entregas_pendientes.xlsx
+++ b/Archivos_xlsx/entregas_pendientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yusti\OneDrive\Escritorio\Prueba Tecnica\PruebaTecnica\Archivos_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B52140-F4EB-47D6-9975-A68FC7192490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0481BC-1DCB-4BBC-8BAF-81D999B00DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,76 +51,76 @@
     <t>2025/03/02</t>
   </si>
   <si>
+    <t>Medellin</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>02-03-2025</t>
+  </si>
+  <si>
+    <t>Entregado</t>
+  </si>
+  <si>
+    <t>Marzo 03, 2025</t>
+  </si>
+  <si>
+    <t>Andres Felipe</t>
+  </si>
+  <si>
+    <t>prueba3@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Felipe Yusti            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Andres Giraldo        </t>
+  </si>
+  <si>
+    <t>Devuelto</t>
+  </si>
+  <si>
+    <t>Giraldo Yusti</t>
+  </si>
+  <si>
+    <t>prueba4@yopmail.com</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>Manolo</t>
+  </si>
+  <si>
+    <t>prueba5@yopmail.com</t>
+  </si>
+  <si>
+    <t>prueba6@yopmail.com</t>
+  </si>
+  <si>
+    <t>prueba7@yopmail.com</t>
+  </si>
+  <si>
+    <t>Bogota</t>
+  </si>
+  <si>
+    <t>Barranquilla</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>prueba8@yopmail.com</t>
+  </si>
+  <si>
     <t>prueba1@yopmail.com</t>
   </si>
   <si>
-    <t>Medellin</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
-    <t>02-03-2025</t>
-  </si>
-  <si>
     <t>prueba2@yopmail.com</t>
-  </si>
-  <si>
-    <t>Entregado</t>
-  </si>
-  <si>
-    <t>Marzo 03, 2025</t>
-  </si>
-  <si>
-    <t>Andres Felipe</t>
-  </si>
-  <si>
-    <t>prueba3@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            Felipe Yusti            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Andres Giraldo        </t>
-  </si>
-  <si>
-    <t>Devuelto</t>
-  </si>
-  <si>
-    <t>Giraldo Yusti</t>
-  </si>
-  <si>
-    <t>prueba4@yopmail.com</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>Miranda</t>
-  </si>
-  <si>
-    <t>Manolo</t>
-  </si>
-  <si>
-    <t>prueba5@yopmail.com</t>
-  </si>
-  <si>
-    <t>prueba6@yopmail.com</t>
-  </si>
-  <si>
-    <t>prueba7@yopmail.com</t>
-  </si>
-  <si>
-    <t>Bogota</t>
-  </si>
-  <si>
-    <t>Barranquilla</t>
-  </si>
-  <si>
-    <t>Sara</t>
-  </si>
-  <si>
-    <t>prueba8@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,16 +529,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="9">
         <v>200000.55554999999</v>
@@ -549,19 +549,19 @@
         <v>1235</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="G3" s="8">
         <v>300000.66666599998</v>
@@ -572,19 +572,19 @@
         <v>1236</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="7">
         <v>400000.77776999999</v>
@@ -598,16 +598,16 @@
         <v>45718</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="G5" s="7">
         <v>500000.88887999998</v>
@@ -621,16 +621,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="9">
         <v>200000.55554999999</v>
@@ -644,16 +644,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="9">
         <v>200000.55554999999</v>
@@ -667,16 +667,16 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G8" s="9">
         <v>200000.55554999999</v>
@@ -690,16 +690,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1">
         <v>200000.1</v>

</xml_diff>